<commit_message>
Add: List Service & Mapper
</commit_message>
<xml_diff>
--- a/Community 테이블 명세 양식.xlsx
+++ b/Community 테이블 명세 양식.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\505-14\Desktop\project\CommunityWorks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bizwork\workspace\Community_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -922,6 +922,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -951,12 +957,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,7 +1241,7 @@
   <dimension ref="B1:S19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2379,56 +2379,56 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="11"/>
-      <c r="O14" s="29" t="s">
+      <c r="O14" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="31"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="33"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="14"/>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="33"/>
-      <c r="O15" s="22" t="s">
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="23"/>
+      <c r="O15" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="24"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="26"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="25"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="24"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="26"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="26"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="30"/>
     </row>
     <row r="18" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O18" s="20"/>
@@ -3569,36 +3569,36 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="29" t="s">
+      <c r="O14" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="31"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="33"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O15" s="22" t="s">
+      <c r="O15" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="24"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="26"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="25"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="24"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="26"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="26"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add: 글 삭제  구현(Update로 Delete 칼럼 값 변경)
</commit_message>
<xml_diff>
--- a/Community 테이블 명세 양식.xlsx
+++ b/Community 테이블 명세 양식.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="114">
   <si>
     <t>테이블 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -91,10 +91,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>조회수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>숫자(자동부여)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -192,10 +188,6 @@
   </si>
   <si>
     <t>숫자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>board_delete</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -478,6 +470,21 @@
   </si>
   <si>
     <t>VARCHAR(20)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>board_delete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조회수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALTER TABLE 자식테이블
+ADD CONSTRAINT 제약조건(외래키)이름
+FOREIGN KEY (자식칼럼)
+REFERENCES 부모테이블(부모칼럼)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1240,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1933,7 +1940,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>7</v>
@@ -1945,19 +1952,19 @@
         <v>9</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -1965,33 +1972,33 @@
         <v>10</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="19"/>
       <c r="O3" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="15">
         <v>1</v>
@@ -2005,35 +2012,35 @@
     </row>
     <row r="4" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="15">
@@ -2049,19 +2056,19 @@
     <row r="5" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="9"/>
       <c r="C5" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2071,7 +2078,7 @@
       <c r="M5" s="11"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q5" s="15">
         <v>2</v>
@@ -2086,19 +2093,19 @@
     <row r="6" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="9"/>
       <c r="C6" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -2124,13 +2131,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -2141,7 +2148,7 @@
       <c r="M7" s="12"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q7" s="15">
         <v>3</v>
@@ -2159,13 +2166,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -2192,16 +2199,16 @@
         <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -2211,7 +2218,7 @@
       <c r="M9" s="12"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q9" s="15">
         <v>4</v>
@@ -2229,16 +2236,16 @@
         <v>15</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -2261,29 +2268,29 @@
     <row r="11" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9"/>
       <c r="C11" s="7" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="12"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q11" s="15">
         <v>5</v>
@@ -2298,16 +2305,16 @@
     <row r="12" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9"/>
       <c r="C12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
@@ -2331,24 +2338,24 @@
     <row r="13" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="9"/>
       <c r="C13" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -2357,30 +2364,30 @@
     <row r="14" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="9"/>
       <c r="C14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="11"/>
       <c r="O14" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
@@ -2390,16 +2397,16 @@
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="14"/>
       <c r="C15" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D15" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>110</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>112</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
@@ -2409,7 +2416,7 @@
       <c r="L15" s="22"/>
       <c r="M15" s="23"/>
       <c r="O15" s="24" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="P15" s="25"/>
       <c r="Q15" s="25"/>
@@ -3153,7 +3160,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>7</v>
@@ -3165,39 +3172,39 @@
         <v>9</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -3205,13 +3212,13 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="15">
         <v>1</v>
@@ -3225,33 +3232,33 @@
     </row>
     <row r="4" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="11"/>
       <c r="O4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="15">
@@ -3267,19 +3274,19 @@
     <row r="5" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="9"/>
       <c r="C5" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -3289,7 +3296,7 @@
       <c r="M5" s="11"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q5" s="15">
         <v>2</v>
@@ -3304,19 +3311,19 @@
     <row r="6" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="9"/>
       <c r="C6" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -3339,16 +3346,16 @@
     <row r="7" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9"/>
       <c r="C7" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -3359,7 +3366,7 @@
       <c r="M7" s="12"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q7" s="15">
         <v>3</v>
@@ -3374,16 +3381,16 @@
     <row r="8" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9"/>
       <c r="C8" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -3407,19 +3414,19 @@
     <row r="9" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9"/>
       <c r="C9" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -3429,7 +3436,7 @@
       <c r="M9" s="12"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="15">
         <v>4</v>
@@ -3444,24 +3451,24 @@
     <row r="10" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9"/>
       <c r="C10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -3481,31 +3488,31 @@
     <row r="11" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9"/>
       <c r="C11" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="12"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q11" s="15">
         <v>5</v>
@@ -3570,7 +3577,7 @@
       <c r="L14" s="16"/>
       <c r="M14" s="17"/>
       <c r="O14" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
@@ -3579,7 +3586,7 @@
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O15" s="24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P15" s="25"/>
       <c r="Q15" s="25"/>

</xml_diff>

<commit_message>
Add: Get Nickname With Join Table
</commit_message>
<xml_diff>
--- a/Community 테이블 명세 양식.xlsx
+++ b/Community 테이블 명세 양식.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="게시판 테이블 명세서" sheetId="1" r:id="rId1"/>
@@ -1247,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O15" sqref="O15:S17"/>
     </sheetView>
   </sheetViews>
@@ -2467,7 +2467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add: 게시판 생성 with Ajax
</commit_message>
<xml_diff>
--- a/Community 테이블 명세 양식.xlsx
+++ b/Community 테이블 명세 양식.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\community_workspace\CommunityWorks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sif\Community_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -749,31 +749,31 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>EQUI JOIN으로 유저 아이디 가져오기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESULT MAP으로 카테고리 목록 가져오기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tbl_board_info</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(bi_id)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tbl_category</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(cate_id)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>LEFT JOIN으로 게시판 이름 가져오기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EQUI JOIN으로 유저 아이디 가져오기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RESULT MAP으로 카테고리 목록 가져오기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tbl_board_info</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(bi_id)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tbl_category</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(cate_id)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1231,6 +1231,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1251,21 +1266,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2657,36 +2657,36 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="31" t="s">
+      <c r="O14" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="27"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="30"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3531,7 +3531,7 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="34"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -3758,36 +3758,36 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="31" t="s">
+      <c r="O14" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="27"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="30"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4843,13 +4843,13 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="11"/>
-      <c r="O14" s="31" t="s">
+      <c r="O14" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="14"/>
@@ -4864,27 +4864,27 @@
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
       <c r="M15" s="23"/>
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="27"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="30"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
     </row>
     <row r="18" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O18" s="20"/>
@@ -5709,7 +5709,7 @@
       <c r="L4" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="25" t="s">
         <v>186</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -5969,36 +5969,36 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="31" t="s">
+      <c r="O14" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="27"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="30"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6844,13 +6844,13 @@
         <v>182</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="M5" s="11" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="6" t="s">
@@ -6895,7 +6895,7 @@
         <v>157</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -7170,13 +7170,13 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="11"/>
-      <c r="O14" s="31" t="s">
+      <c r="O14" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="14"/>
@@ -7199,35 +7199,35 @@
         <v>181</v>
       </c>
       <c r="K15" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="L15" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="L15" s="22" t="s">
-        <v>193</v>
-      </c>
       <c r="M15" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="O15" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="O15" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="27"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="30"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
     </row>
     <row r="18" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O18" s="20"/>
@@ -8375,36 +8375,36 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="31" t="s">
+      <c r="O14" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O16" s="27"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="15:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="30"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add: Spring Security + 무한댓글 구현 & CSS
</commit_message>
<xml_diff>
--- a/Community 테이블 명세 양식.xlsx
+++ b/Community 테이블 명세 양식.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="199">
   <si>
     <t>테이블 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -685,10 +685,6 @@
   </si>
   <si>
     <t>INT</t>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>INT</t>
@@ -1266,6 +1262,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1295,9 +1294,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3324,7 +3320,7 @@
         <v>138</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -4193,7 +4189,7 @@
     </row>
     <row r="3" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>142</v>
@@ -5187,7 +5183,7 @@
         <v>158</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -5350,9 +5346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6089,7 +6083,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
@@ -6117,16 +6111,16 @@
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>24</v>
@@ -6141,13 +6135,13 @@
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="9"/>
       <c r="C6" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>22</v>
@@ -6165,13 +6159,13 @@
     <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9"/>
       <c r="C7" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>22</v>
@@ -6207,7 +6201,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -6232,8 +6226,8 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="36" t="s">
-        <v>191</v>
+      <c r="M9" s="26" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -6248,7 +6242,7 @@
         <v>169</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>24</v>
@@ -6411,13 +6405,13 @@
     <row r="17" spans="2:19" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9"/>
       <c r="C17" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>135</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>171</v>
@@ -6429,7 +6423,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="2:19" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -7206,7 +7200,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>135</v>
@@ -7232,13 +7226,13 @@
         <v>141</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="9"/>
       <c r="C5" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>61</v>
@@ -7271,10 +7265,10 @@
         <v>165</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>172</v>
+        <v>20</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -7292,13 +7286,13 @@
         <v>163</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -7319,10 +7313,10 @@
         <v>166</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -7361,20 +7355,20 @@
         <v>67</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -7663,36 +7657,36 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="B15" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="32"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add: Category Delete. Update: Table & Excel
</commit_message>
<xml_diff>
--- a/Community 테이블 명세 양식.xlsx
+++ b/Community 테이블 명세 양식.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Works\workspace\CommunityWorks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sif\Community_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A972D3B-A3FC-49BD-8514-F512F0A78D23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="유저 테이블" sheetId="7" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="200">
   <si>
     <t>테이블 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -743,6 +742,23 @@
   </si>
   <si>
     <t>board_depth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 정보 테이블</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>board_order</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmt_order</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON DELETE CASCADE
+게시판 삭제되면 연결된 카테고리 삭제</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -751,31 +767,18 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ON DELETE CASCADE
+부모글 삭제되면 댓글 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON DELETE CASCADE
+유저 삭제되면 유저권한도 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>EQUI JOIN으로 유저 아이디 가져오기
 작성자 계정이 삭제돼도 쓴 글은 남아있도록 외래키 설정하지 않음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>카테고리가 삭제돼도 쓴 글은 남아있도록 외래키 설정하지 않음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ON DELETE CASCADE
-부모글 삭제돼면 댓글 삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ON DELETE CASCADE
-게시판 삭제돼면 연결된 카테고리 삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ON DELETE CASCADE
-유저 삭제돼면 유저권한도 삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시판 정보 테이블</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -783,22 +786,36 @@
 ADD CONSTRAINT 제약조건(외래키)이름
 FOREIGN KEY (자식칼럼)
 REFERENCES 부모테이블(부모칼럼)
-ON DELETE CASCADE(부모 데이터 삭제시 연결된 자식 데이터 삭제)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>board_order</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cmt_order</t>
+ON DELETE
+Cascade : 부모 데이터 삭제 시 자식 데이터도 삭제 
+Set null : 부모 데이터 삭제 시 자식 테이블의 참조 컬럼을 Null로 업데이트
+Set default : 부모 데이터 삭제 시 자식 테이블의 참조 컬럼을 Default 값으로 업데이트
+Restrict : 자식 테이블이 참조하고 있을 경우, 데이터 삭제 불가
+No Action : Restrict와 동일, 옵션을 지정하지 않았을 경우 자동으로 선택된다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK_CATE_BOARD_board_category</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tbl_category</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cate_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON DELETE SET DEFAULT
+카테고리 삭제 시 DEFAULT 값으로</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
@@ -856,7 +873,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1170,13 +1187,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1270,22 +1318,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1567,10 +1621,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2547,7 +2601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -3313,7 +3367,7 @@
         <v>136</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -3473,7 +3527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -4182,7 +4236,7 @@
     </row>
     <row r="3" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>140</v>
@@ -4411,7 +4465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -5176,7 +5230,7 @@
         <v>156</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -5336,10 +5390,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6134,7 +6188,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>22</v>
@@ -6194,7 +6248,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="25" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -6220,7 +6274,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="26" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -6412,11 +6466,17 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="11" t="s">
-        <v>189</v>
+      <c r="J17" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="2:19" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6454,7 +6514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -7219,7 +7279,7 @@
         <v>139</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -7279,7 +7339,7 @@
         <v>161</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>170</v>
@@ -7467,10 +7527,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7659,32 +7721,53 @@
       <c r="F14" s="29"/>
     </row>
     <row r="15" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
+      <c r="B15" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="33"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+    </row>
+    <row r="18" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="30"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+    </row>
+    <row r="19" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="30"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="20" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F17"/>
+    <mergeCell ref="B15:F20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update: SQL(EQUI JOIN -> LEFT JOIN)
</commit_message>
<xml_diff>
--- a/Community 테이블 명세 양식.xlsx
+++ b/Community 테이블 명세 양식.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="유저 테이블" sheetId="7" r:id="rId1"/>
@@ -1315,9 +1315,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1325,6 +1322,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1624,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5393,7 +5393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7530,9 +7530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:F20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7721,37 +7719,37 @@
       <c r="F14" s="29"/>
     </row>
     <row r="15" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="30"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
       <c r="F16" s="35"/>
     </row>
     <row r="17" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="30"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="35"/>
     </row>
     <row r="18" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="30"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
       <c r="F18" s="35"/>
     </row>
     <row r="19" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="30"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>

</xml_diff>